<commit_message>
fuzzy_4 and test result
</commit_message>
<xml_diff>
--- a/hammer-colombo/fuzzy-examples-set/test.xlsx
+++ b/hammer-colombo/fuzzy-examples-set/test.xlsx
@@ -729,8 +729,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:P20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -946,20 +946,36 @@
       <c r="F6" s="12">
         <v>1</v>
       </c>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="13"/>
+      <c r="G6" s="12">
+        <v>1</v>
+      </c>
+      <c r="H6" s="12">
+        <v>1</v>
+      </c>
+      <c r="I6" s="12">
+        <v>1</v>
+      </c>
+      <c r="J6" s="12">
+        <v>1</v>
+      </c>
       <c r="K6" s="12">
         <v>0.25</v>
       </c>
       <c r="L6" s="12">
         <v>0.25</v>
       </c>
-      <c r="M6" s="7"/>
-      <c r="N6" s="7"/>
-      <c r="O6" s="7"/>
-      <c r="P6" s="13"/>
+      <c r="M6" s="12">
+        <v>0.25</v>
+      </c>
+      <c r="N6" s="12">
+        <v>0.25</v>
+      </c>
+      <c r="O6" s="12">
+        <v>0.25</v>
+      </c>
+      <c r="P6" s="12">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">

</xml_diff>

<commit_message>
create base line 8
</commit_message>
<xml_diff>
--- a/hammer-colombo/fuzzy-examples-set/test.xlsx
+++ b/hammer-colombo/fuzzy-examples-set/test.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4820" yWindow="500" windowWidth="25460" windowHeight="13600" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="4820" yWindow="460" windowWidth="25460" windowHeight="13600" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="5" r:id="rId1"/>
@@ -3047,8 +3047,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:T29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3397,11 +3397,19 @@
       <c r="C11" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="7"/>
-      <c r="E11" s="62"/>
+      <c r="D11" s="7">
+        <v>1</v>
+      </c>
+      <c r="E11" s="62">
+        <v>0</v>
+      </c>
       <c r="F11" s="10"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="62"/>
+      <c r="G11" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="H11" s="62">
+        <v>0</v>
+      </c>
       <c r="I11" s="10"/>
       <c r="K11" s="76">
         <v>1</v>
@@ -3423,11 +3431,19 @@
       <c r="C12" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="7"/>
-      <c r="E12" s="62"/>
+      <c r="D12" s="7">
+        <v>1</v>
+      </c>
+      <c r="E12" s="62">
+        <v>1</v>
+      </c>
       <c r="F12" s="10"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="62"/>
+      <c r="G12" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="H12" s="62">
+        <v>1</v>
+      </c>
       <c r="I12" s="10"/>
       <c r="K12" s="76">
         <v>1</v>
@@ -3471,11 +3487,11 @@
     <row r="14" spans="2:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D14" s="34">
         <f>AVERAGE(D5:D13)</f>
-        <v>0.66666666666666663</v>
+        <v>0.75</v>
       </c>
       <c r="E14" s="64">
         <f t="shared" ref="E14:F14" si="0">AVERAGE(E5:E13)</f>
-        <v>0</v>
+        <v>0.125</v>
       </c>
       <c r="F14" s="38" t="e">
         <f t="shared" si="0"/>
@@ -3483,11 +3499,11 @@
       </c>
       <c r="G14" s="34">
         <f>AVERAGE(G5:G13)</f>
-        <v>6.6666666666666666E-2</v>
+        <v>0.11250000000000002</v>
       </c>
       <c r="H14" s="64">
         <f t="shared" ref="H14:I14" si="1">AVERAGE(H5:H13)</f>
-        <v>0</v>
+        <v>0.125</v>
       </c>
       <c r="I14" s="38" t="e">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
create base line 9
</commit_message>
<xml_diff>
--- a/hammer-colombo/fuzzy-examples-set/test.xlsx
+++ b/hammer-colombo/fuzzy-examples-set/test.xlsx
@@ -3047,8 +3047,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:T29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3465,11 +3465,19 @@
       <c r="C13" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="27"/>
-      <c r="E13" s="63"/>
+      <c r="D13" s="27">
+        <v>1</v>
+      </c>
+      <c r="E13" s="63">
+        <v>1</v>
+      </c>
       <c r="F13" s="32"/>
-      <c r="G13" s="27"/>
-      <c r="H13" s="63"/>
+      <c r="G13" s="27">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="H13" s="63">
+        <v>1</v>
+      </c>
       <c r="I13" s="32"/>
       <c r="K13" s="78">
         <v>1</v>
@@ -3487,11 +3495,11 @@
     <row r="14" spans="2:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D14" s="34">
         <f>AVERAGE(D5:D13)</f>
-        <v>0.75</v>
+        <v>0.77777777777777779</v>
       </c>
       <c r="E14" s="64">
         <f t="shared" ref="E14:F14" si="0">AVERAGE(E5:E13)</f>
-        <v>0.125</v>
+        <v>0.22222222222222221</v>
       </c>
       <c r="F14" s="38" t="e">
         <f t="shared" si="0"/>
@@ -3499,11 +3507,11 @@
       </c>
       <c r="G14" s="34">
         <f>AVERAGE(G5:G13)</f>
-        <v>0.11250000000000002</v>
+        <v>0.13703333333333334</v>
       </c>
       <c r="H14" s="64">
         <f t="shared" ref="H14:I14" si="1">AVERAGE(H5:H13)</f>
-        <v>0.125</v>
+        <v>0.22222222222222221</v>
       </c>
       <c r="I14" s="38" t="e">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
create base line apache solr
</commit_message>
<xml_diff>
--- a/hammer-colombo/fuzzy-examples-set/test.xlsx
+++ b/hammer-colombo/fuzzy-examples-set/test.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4820" yWindow="460" windowWidth="25460" windowHeight="13600" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="560" yWindow="1440" windowWidth="25460" windowHeight="13600" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="5" r:id="rId1"/>
@@ -373,7 +373,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -450,6 +450,14 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -917,10 +925,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -965,7 +974,37 @@
     <xf numFmtId="10" fontId="10" fillId="9" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="10" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="6" fillId="11" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="6" fillId="11" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="10" fillId="11" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="6" fillId="2" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="6" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="6" fillId="8" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="6" fillId="8" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="6" fillId="8" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="6" fillId="8" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="10" fillId="10" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="10" fillId="10" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -983,6 +1022,12 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -990,24 +1035,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1022,12 +1049,15 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="6" fillId="11" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="6" fillId="11" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="10" fillId="11" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1037,33 +1067,13 @@
     <xf numFmtId="0" fontId="9" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="6" fillId="2" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="6" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="6" fillId="8" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="6" fillId="8" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="6" fillId="8" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="6" fillId="8" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="10" fillId="10" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="10" fillId="10" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Collegamento ipertestuale" xfId="2" builtinId="8"/>
+    <cellStyle name="Collegamento ipertestuale visitato" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
     <cellStyle name="Percentuale" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -1346,7 +1356,7 @@
   <dimension ref="B1:AM26"/>
   <sheetViews>
     <sheetView topLeftCell="Q1" zoomScale="101" workbookViewId="0">
-      <selection activeCell="V1" sqref="V1:AM1"/>
+      <selection activeCell="W4" sqref="W4:W13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1366,92 +1376,92 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:39" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D1" s="49" t="s">
+      <c r="D1" s="58" t="s">
         <v>46</v>
       </c>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
-      <c r="I1" s="49"/>
-      <c r="J1" s="49"/>
-      <c r="K1" s="49"/>
-      <c r="L1" s="49"/>
-      <c r="M1" s="49"/>
-      <c r="N1" s="49"/>
-      <c r="O1" s="49"/>
-      <c r="P1" s="49"/>
-      <c r="Q1" s="49"/>
-      <c r="R1" s="49"/>
-      <c r="S1" s="49"/>
-      <c r="T1" s="49"/>
-      <c r="U1" s="49"/>
-      <c r="V1" s="51" t="s">
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
+      <c r="J1" s="58"/>
+      <c r="K1" s="58"/>
+      <c r="L1" s="58"/>
+      <c r="M1" s="58"/>
+      <c r="N1" s="58"/>
+      <c r="O1" s="58"/>
+      <c r="P1" s="58"/>
+      <c r="Q1" s="58"/>
+      <c r="R1" s="58"/>
+      <c r="S1" s="58"/>
+      <c r="T1" s="58"/>
+      <c r="U1" s="58"/>
+      <c r="V1" s="60" t="s">
         <v>47</v>
       </c>
-      <c r="W1" s="52"/>
-      <c r="X1" s="52"/>
-      <c r="Y1" s="52"/>
-      <c r="Z1" s="52"/>
-      <c r="AA1" s="52"/>
-      <c r="AB1" s="52"/>
-      <c r="AC1" s="52"/>
-      <c r="AD1" s="52"/>
-      <c r="AE1" s="52"/>
-      <c r="AF1" s="52"/>
-      <c r="AG1" s="52"/>
-      <c r="AH1" s="52"/>
-      <c r="AI1" s="52"/>
-      <c r="AJ1" s="52"/>
-      <c r="AK1" s="52"/>
-      <c r="AL1" s="52"/>
-      <c r="AM1" s="53"/>
+      <c r="W1" s="61"/>
+      <c r="X1" s="61"/>
+      <c r="Y1" s="61"/>
+      <c r="Z1" s="61"/>
+      <c r="AA1" s="61"/>
+      <c r="AB1" s="61"/>
+      <c r="AC1" s="61"/>
+      <c r="AD1" s="61"/>
+      <c r="AE1" s="61"/>
+      <c r="AF1" s="61"/>
+      <c r="AG1" s="61"/>
+      <c r="AH1" s="61"/>
+      <c r="AI1" s="61"/>
+      <c r="AJ1" s="61"/>
+      <c r="AK1" s="61"/>
+      <c r="AL1" s="61"/>
+      <c r="AM1" s="62"/>
     </row>
     <row r="2" spans="2:39" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D2" s="41" t="s">
+      <c r="D2" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="42"/>
-      <c r="J2" s="42"/>
-      <c r="K2" s="42"/>
-      <c r="L2" s="43"/>
-      <c r="M2" s="44" t="s">
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="64"/>
+      <c r="K2" s="64"/>
+      <c r="L2" s="65"/>
+      <c r="M2" s="66" t="s">
         <v>25</v>
       </c>
-      <c r="N2" s="45"/>
-      <c r="O2" s="45"/>
-      <c r="P2" s="45"/>
-      <c r="Q2" s="45"/>
-      <c r="R2" s="45"/>
-      <c r="S2" s="45"/>
-      <c r="T2" s="45"/>
-      <c r="U2" s="46"/>
-      <c r="V2" s="41" t="s">
+      <c r="N2" s="67"/>
+      <c r="O2" s="67"/>
+      <c r="P2" s="67"/>
+      <c r="Q2" s="67"/>
+      <c r="R2" s="67"/>
+      <c r="S2" s="67"/>
+      <c r="T2" s="67"/>
+      <c r="U2" s="70"/>
+      <c r="V2" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="W2" s="42"/>
-      <c r="X2" s="42"/>
-      <c r="Y2" s="42"/>
-      <c r="Z2" s="42"/>
-      <c r="AA2" s="42"/>
-      <c r="AB2" s="42"/>
-      <c r="AC2" s="42"/>
-      <c r="AD2" s="43"/>
-      <c r="AE2" s="44" t="s">
+      <c r="W2" s="64"/>
+      <c r="X2" s="64"/>
+      <c r="Y2" s="64"/>
+      <c r="Z2" s="64"/>
+      <c r="AA2" s="64"/>
+      <c r="AB2" s="64"/>
+      <c r="AC2" s="64"/>
+      <c r="AD2" s="65"/>
+      <c r="AE2" s="66" t="s">
         <v>25</v>
       </c>
-      <c r="AF2" s="45"/>
-      <c r="AG2" s="45"/>
-      <c r="AH2" s="45"/>
-      <c r="AI2" s="45"/>
-      <c r="AJ2" s="45"/>
-      <c r="AK2" s="45"/>
-      <c r="AL2" s="45"/>
-      <c r="AM2" s="54"/>
+      <c r="AF2" s="67"/>
+      <c r="AG2" s="67"/>
+      <c r="AH2" s="67"/>
+      <c r="AI2" s="67"/>
+      <c r="AJ2" s="67"/>
+      <c r="AK2" s="67"/>
+      <c r="AL2" s="67"/>
+      <c r="AM2" s="68"/>
     </row>
     <row r="3" spans="2:39" x14ac:dyDescent="0.2">
       <c r="B3" s="13" t="s">
@@ -1889,7 +1899,7 @@
       <c r="AD6" s="10">
         <v>1</v>
       </c>
-      <c r="AE6" s="68">
+      <c r="AE6" s="46">
         <v>0</v>
       </c>
       <c r="AF6" s="24">
@@ -1898,7 +1908,7 @@
       <c r="AG6" s="8">
         <v>0.51429999999999998</v>
       </c>
-      <c r="AH6" s="69">
+      <c r="AH6" s="47">
         <v>0</v>
       </c>
       <c r="AI6" s="21">
@@ -1907,7 +1917,7 @@
       <c r="AJ6" s="8">
         <v>0.4854</v>
       </c>
-      <c r="AK6" s="69">
+      <c r="AK6" s="47">
         <v>0</v>
       </c>
       <c r="AL6" s="8">
@@ -2237,7 +2247,7 @@
       <c r="AD9" s="10">
         <v>1</v>
       </c>
-      <c r="AE9" s="68">
+      <c r="AE9" s="46">
         <v>0</v>
       </c>
       <c r="AF9" s="24">
@@ -2246,7 +2256,7 @@
       <c r="AG9" s="8">
         <v>0.5</v>
       </c>
-      <c r="AH9" s="69">
+      <c r="AH9" s="47">
         <v>0</v>
       </c>
       <c r="AI9" s="21">
@@ -2255,7 +2265,7 @@
       <c r="AJ9" s="8">
         <v>0.5</v>
       </c>
-      <c r="AK9" s="69">
+      <c r="AK9" s="47">
         <v>0</v>
       </c>
       <c r="AL9" s="8">
@@ -2353,7 +2363,7 @@
       <c r="AD10" s="10">
         <v>1</v>
       </c>
-      <c r="AE10" s="68">
+      <c r="AE10" s="46">
         <v>0</v>
       </c>
       <c r="AF10" s="24">
@@ -2362,7 +2372,7 @@
       <c r="AG10" s="8">
         <v>0.94740000000000002</v>
       </c>
-      <c r="AH10" s="69">
+      <c r="AH10" s="47">
         <v>0</v>
       </c>
       <c r="AI10" s="21">
@@ -2371,7 +2381,7 @@
       <c r="AJ10" s="8">
         <v>0.94740000000000002</v>
       </c>
-      <c r="AK10" s="69">
+      <c r="AK10" s="47">
         <v>0</v>
       </c>
       <c r="AL10" s="8">
@@ -2760,10 +2770,10 @@
       </c>
     </row>
     <row r="17" spans="2:19" ht="64" x14ac:dyDescent="0.2">
-      <c r="B17" s="50" t="s">
+      <c r="B17" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="50"/>
+      <c r="C17" s="59"/>
       <c r="D17" s="1" t="s">
         <v>0</v>
       </c>
@@ -2782,15 +2792,15 @@
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
-      <c r="M17" s="40"/>
-      <c r="N17" s="40"/>
-      <c r="O17" s="40"/>
-      <c r="P17" s="40" t="s">
+      <c r="M17" s="69"/>
+      <c r="N17" s="69"/>
+      <c r="O17" s="69"/>
+      <c r="P17" s="69" t="s">
         <v>27</v>
       </c>
-      <c r="Q17" s="40"/>
-      <c r="R17" s="40"/>
-      <c r="S17" s="40"/>
+      <c r="Q17" s="69"/>
+      <c r="R17" s="69"/>
+      <c r="S17" s="69"/>
     </row>
     <row r="18" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B18" s="2" t="s">
@@ -2811,17 +2821,17 @@
       <c r="H18" t="s">
         <v>7</v>
       </c>
-      <c r="M18" s="40" t="s">
+      <c r="M18" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="N18" s="40"/>
-      <c r="O18" s="40"/>
-      <c r="P18" s="40">
+      <c r="N18" s="69"/>
+      <c r="O18" s="69"/>
+      <c r="P18" s="69">
         <v>2300</v>
       </c>
-      <c r="Q18" s="40"/>
-      <c r="R18" s="40"/>
-      <c r="S18" s="40"/>
+      <c r="Q18" s="69"/>
+      <c r="R18" s="69"/>
+      <c r="S18" s="69"/>
     </row>
     <row r="19" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B19" s="2" t="s">
@@ -2842,17 +2852,17 @@
       <c r="H19" t="s">
         <v>7</v>
       </c>
-      <c r="M19" s="40" t="s">
+      <c r="M19" s="69" t="s">
         <v>29</v>
       </c>
-      <c r="N19" s="40"/>
-      <c r="O19" s="40"/>
-      <c r="P19" s="40">
+      <c r="N19" s="69"/>
+      <c r="O19" s="69"/>
+      <c r="P19" s="69">
         <v>10180</v>
       </c>
-      <c r="Q19" s="40"/>
-      <c r="R19" s="40"/>
-      <c r="S19" s="40"/>
+      <c r="Q19" s="69"/>
+      <c r="R19" s="69"/>
+      <c r="S19" s="69"/>
     </row>
     <row r="20" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B20" s="2" t="s">
@@ -2873,17 +2883,17 @@
       <c r="H20" t="s">
         <v>7</v>
       </c>
-      <c r="M20" s="40" t="s">
+      <c r="M20" s="69" t="s">
         <v>45</v>
       </c>
-      <c r="N20" s="40"/>
-      <c r="O20" s="40"/>
-      <c r="P20" s="40">
+      <c r="N20" s="69"/>
+      <c r="O20" s="69"/>
+      <c r="P20" s="69">
         <v>4838568</v>
       </c>
-      <c r="Q20" s="40"/>
-      <c r="R20" s="40"/>
-      <c r="S20" s="40"/>
+      <c r="Q20" s="69"/>
+      <c r="R20" s="69"/>
+      <c r="S20" s="69"/>
     </row>
     <row r="21" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B21" s="2" t="s">
@@ -2904,17 +2914,17 @@
       <c r="H21" t="s">
         <v>7</v>
       </c>
-      <c r="M21" s="47" t="s">
+      <c r="M21" s="71" t="s">
         <v>43</v>
       </c>
-      <c r="N21" s="47"/>
-      <c r="O21" s="47"/>
-      <c r="P21" s="48" t="s">
+      <c r="N21" s="71"/>
+      <c r="O21" s="71"/>
+      <c r="P21" s="72" t="s">
         <v>44</v>
       </c>
-      <c r="Q21" s="48"/>
-      <c r="R21" s="48"/>
-      <c r="S21" s="48"/>
+      <c r="Q21" s="72"/>
+      <c r="R21" s="72"/>
+      <c r="S21" s="72"/>
     </row>
     <row r="22" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B22" s="2" t="s">
@@ -3018,13 +3028,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="D1:U1"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="V1:AM1"/>
-    <mergeCell ref="V2:AD2"/>
-    <mergeCell ref="AE2:AM2"/>
-    <mergeCell ref="P17:S17"/>
-    <mergeCell ref="M17:O17"/>
     <mergeCell ref="M19:O19"/>
     <mergeCell ref="M20:O20"/>
     <mergeCell ref="D2:L2"/>
@@ -3035,6 +3038,13 @@
     <mergeCell ref="P20:S20"/>
     <mergeCell ref="P18:S18"/>
     <mergeCell ref="M18:O18"/>
+    <mergeCell ref="D1:U1"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="V1:AM1"/>
+    <mergeCell ref="V2:AD2"/>
+    <mergeCell ref="AE2:AM2"/>
+    <mergeCell ref="P17:S17"/>
+    <mergeCell ref="M17:O17"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="P21" r:id="rId1"/>
@@ -3048,7 +3058,7 @@
   <dimension ref="B1:T29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3071,47 +3081,47 @@
       <c r="N1" s="83"/>
     </row>
     <row r="2" spans="2:20" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D2" s="65" t="s">
+      <c r="D2" s="80" t="s">
         <v>46</v>
       </c>
-      <c r="E2" s="66"/>
-      <c r="F2" s="66"/>
-      <c r="G2" s="66"/>
-      <c r="H2" s="66"/>
-      <c r="I2" s="67"/>
-      <c r="K2" s="65" t="s">
+      <c r="E2" s="81"/>
+      <c r="F2" s="81"/>
+      <c r="G2" s="81"/>
+      <c r="H2" s="81"/>
+      <c r="I2" s="82"/>
+      <c r="K2" s="80" t="s">
         <v>46</v>
       </c>
-      <c r="L2" s="67"/>
-      <c r="M2" s="51" t="s">
+      <c r="L2" s="82"/>
+      <c r="M2" s="60" t="s">
         <v>47</v>
       </c>
-      <c r="N2" s="53"/>
+      <c r="N2" s="62"/>
     </row>
     <row r="3" spans="2:20" ht="49" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D3" s="56" t="s">
+      <c r="D3" s="74" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="57"/>
-      <c r="F3" s="58"/>
-      <c r="G3" s="70" t="s">
+      <c r="E3" s="75"/>
+      <c r="F3" s="76"/>
+      <c r="G3" s="77" t="s">
         <v>25</v>
       </c>
-      <c r="H3" s="71"/>
-      <c r="I3" s="72"/>
-      <c r="K3" s="59" t="s">
+      <c r="H3" s="78"/>
+      <c r="I3" s="79"/>
+      <c r="K3" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="L3" s="73" t="s">
+      <c r="L3" s="48" t="s">
         <v>25</v>
       </c>
-      <c r="M3" s="59" t="s">
+      <c r="M3" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="N3" s="73" t="s">
+      <c r="N3" s="48" t="s">
         <v>25</v>
       </c>
-      <c r="O3" s="82" t="s">
+      <c r="O3" s="57" t="s">
         <v>14</v>
       </c>
       <c r="P3" s="1" t="s">
@@ -3140,31 +3150,31 @@
       <c r="D4" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="E4" s="61" t="s">
+      <c r="E4" s="42" t="s">
         <v>112</v>
       </c>
-      <c r="F4" s="60" t="s">
+      <c r="F4" s="41" t="s">
         <v>106</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="H4" s="61" t="s">
+      <c r="H4" s="42" t="s">
         <v>112</v>
       </c>
-      <c r="I4" s="60" t="s">
+      <c r="I4" s="41" t="s">
         <v>106</v>
       </c>
-      <c r="K4" s="74" t="s">
+      <c r="K4" s="49" t="s">
         <v>109</v>
       </c>
-      <c r="L4" s="75" t="s">
+      <c r="L4" s="50" t="s">
         <v>109</v>
       </c>
-      <c r="M4" s="74" t="s">
+      <c r="M4" s="49" t="s">
         <v>109</v>
       </c>
-      <c r="N4" s="75" t="s">
+      <c r="N4" s="50" t="s">
         <v>109</v>
       </c>
       <c r="O4" s="2" t="s">
@@ -3196,28 +3206,32 @@
       <c r="D5" s="7">
         <v>0</v>
       </c>
-      <c r="E5" s="62">
+      <c r="E5" s="43">
         <v>0</v>
       </c>
-      <c r="F5" s="10"/>
+      <c r="F5" s="10">
+        <v>1</v>
+      </c>
       <c r="G5" s="7">
         <v>0</v>
       </c>
-      <c r="H5" s="62">
+      <c r="H5" s="43">
         <v>0</v>
       </c>
-      <c r="I5" s="10"/>
-      <c r="K5" s="76">
+      <c r="I5" s="10">
+        <v>0.22090000000000001</v>
+      </c>
+      <c r="K5" s="51">
         <v>0.1333</v>
       </c>
-      <c r="L5" s="77">
+      <c r="L5" s="52">
         <v>0.66669999999999996</v>
       </c>
-      <c r="M5" s="76">
-        <v>0.1333</v>
-      </c>
-      <c r="N5" s="77">
-        <v>0.66669999999999996</v>
+      <c r="M5" s="51">
+        <v>1</v>
+      </c>
+      <c r="N5" s="52">
+        <v>0.5</v>
       </c>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.2">
@@ -3230,28 +3244,32 @@
       <c r="D6" s="7">
         <v>1</v>
       </c>
-      <c r="E6" s="62">
+      <c r="E6" s="43">
         <v>0</v>
       </c>
-      <c r="F6" s="10"/>
+      <c r="F6" s="10">
+        <v>1</v>
+      </c>
       <c r="G6" s="7">
         <v>0.05</v>
       </c>
-      <c r="H6" s="62">
+      <c r="H6" s="43">
         <v>0</v>
       </c>
-      <c r="I6" s="10"/>
-      <c r="K6" s="76">
-        <v>1</v>
-      </c>
-      <c r="L6" s="77">
+      <c r="I6" s="10">
+        <v>1.9599999999999999E-2</v>
+      </c>
+      <c r="K6" s="51">
+        <v>1</v>
+      </c>
+      <c r="L6" s="52">
         <v>0.5</v>
       </c>
-      <c r="M6" s="76">
-        <v>1</v>
-      </c>
-      <c r="N6" s="77">
-        <v>0.5</v>
+      <c r="M6" s="51">
+        <v>1</v>
+      </c>
+      <c r="N6" s="52">
+        <v>0.89910000000000001</v>
       </c>
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.2">
@@ -3264,28 +3282,32 @@
       <c r="D7" s="7">
         <v>1</v>
       </c>
-      <c r="E7" s="62">
+      <c r="E7" s="43">
         <v>0</v>
       </c>
-      <c r="F7" s="10"/>
+      <c r="F7" s="10">
+        <v>1</v>
+      </c>
       <c r="G7" s="7">
         <v>0.15</v>
       </c>
-      <c r="H7" s="62">
+      <c r="H7" s="43">
         <v>0</v>
       </c>
-      <c r="I7" s="10"/>
-      <c r="K7" s="76">
-        <v>1</v>
-      </c>
-      <c r="L7" s="77">
+      <c r="I7" s="10">
+        <v>0.25</v>
+      </c>
+      <c r="K7" s="51">
+        <v>1</v>
+      </c>
+      <c r="L7" s="52">
         <v>0.75</v>
       </c>
-      <c r="M7" s="76">
-        <v>1</v>
-      </c>
-      <c r="N7" s="77">
-        <v>0.75</v>
+      <c r="M7" s="51">
+        <v>1</v>
+      </c>
+      <c r="N7" s="52">
+        <v>0.51429999999999998</v>
       </c>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.2">
@@ -3298,28 +3320,28 @@
       <c r="D8" s="7">
         <v>0</v>
       </c>
-      <c r="E8" s="62">
+      <c r="E8" s="43">
         <v>0</v>
       </c>
       <c r="F8" s="10"/>
       <c r="G8" s="7">
         <v>0</v>
       </c>
-      <c r="H8" s="62">
+      <c r="H8" s="43">
         <v>0</v>
       </c>
       <c r="I8" s="10"/>
-      <c r="K8" s="76">
+      <c r="K8" s="51">
         <v>0.66669999999999996</v>
       </c>
-      <c r="L8" s="77">
+      <c r="L8" s="52">
         <v>0.1333</v>
       </c>
-      <c r="M8" s="76">
-        <v>0.66669999999999996</v>
-      </c>
-      <c r="N8" s="77">
-        <v>0.1333</v>
+      <c r="M8" s="51">
+        <v>1</v>
+      </c>
+      <c r="N8" s="52">
+        <v>0.1439</v>
       </c>
     </row>
     <row r="9" spans="2:20" x14ac:dyDescent="0.2">
@@ -3332,27 +3354,27 @@
       <c r="D9" s="7">
         <v>1</v>
       </c>
-      <c r="E9" s="62">
+      <c r="E9" s="43">
         <v>0</v>
       </c>
       <c r="F9" s="10"/>
       <c r="G9" s="7">
         <v>0.05</v>
       </c>
-      <c r="H9" s="62">
+      <c r="H9" s="43">
         <v>0</v>
       </c>
       <c r="I9" s="10"/>
-      <c r="K9" s="76">
-        <v>1</v>
-      </c>
-      <c r="L9" s="77">
-        <v>1</v>
-      </c>
-      <c r="M9" s="76">
-        <v>1</v>
-      </c>
-      <c r="N9" s="77">
+      <c r="K9" s="51">
+        <v>1</v>
+      </c>
+      <c r="L9" s="52">
+        <v>1</v>
+      </c>
+      <c r="M9" s="51">
+        <v>1</v>
+      </c>
+      <c r="N9" s="52">
         <v>1</v>
       </c>
     </row>
@@ -3366,28 +3388,28 @@
       <c r="D10" s="7">
         <v>1</v>
       </c>
-      <c r="E10" s="62">
+      <c r="E10" s="43">
         <v>0</v>
       </c>
       <c r="F10" s="10"/>
       <c r="G10" s="7">
         <v>0.15</v>
       </c>
-      <c r="H10" s="62">
+      <c r="H10" s="43">
         <v>0</v>
       </c>
       <c r="I10" s="10"/>
-      <c r="K10" s="76">
-        <v>1</v>
-      </c>
-      <c r="L10" s="77">
+      <c r="K10" s="51">
+        <v>1</v>
+      </c>
+      <c r="L10" s="52">
         <v>0.33329999999999999</v>
       </c>
-      <c r="M10" s="76">
-        <v>1</v>
-      </c>
-      <c r="N10" s="77">
-        <v>0.33329999999999999</v>
+      <c r="M10" s="51">
+        <v>1</v>
+      </c>
+      <c r="N10" s="52">
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="2:20" x14ac:dyDescent="0.2">
@@ -3400,27 +3422,27 @@
       <c r="D11" s="7">
         <v>1</v>
       </c>
-      <c r="E11" s="62">
+      <c r="E11" s="43">
         <v>0</v>
       </c>
       <c r="F11" s="10"/>
       <c r="G11" s="7">
         <v>0.2</v>
       </c>
-      <c r="H11" s="62">
+      <c r="H11" s="43">
         <v>0</v>
       </c>
       <c r="I11" s="10"/>
-      <c r="K11" s="76">
-        <v>1</v>
-      </c>
-      <c r="L11" s="77">
-        <v>1</v>
-      </c>
-      <c r="M11" s="76">
-        <v>1</v>
-      </c>
-      <c r="N11" s="77">
+      <c r="K11" s="51">
+        <v>1</v>
+      </c>
+      <c r="L11" s="52">
+        <v>1</v>
+      </c>
+      <c r="M11" s="51">
+        <v>1</v>
+      </c>
+      <c r="N11" s="52">
         <v>1</v>
       </c>
     </row>
@@ -3434,27 +3456,27 @@
       <c r="D12" s="7">
         <v>1</v>
       </c>
-      <c r="E12" s="62">
+      <c r="E12" s="43">
         <v>1</v>
       </c>
       <c r="F12" s="10"/>
       <c r="G12" s="7">
         <v>0.3</v>
       </c>
-      <c r="H12" s="62">
+      <c r="H12" s="43">
         <v>1</v>
       </c>
       <c r="I12" s="10"/>
-      <c r="K12" s="76">
-        <v>1</v>
-      </c>
-      <c r="L12" s="77">
+      <c r="K12" s="51">
+        <v>1</v>
+      </c>
+      <c r="L12" s="52">
         <v>0.5</v>
       </c>
-      <c r="M12" s="76">
-        <v>1</v>
-      </c>
-      <c r="N12" s="77">
+      <c r="M12" s="51">
+        <v>1</v>
+      </c>
+      <c r="N12" s="52">
         <v>0.5</v>
       </c>
     </row>
@@ -3468,28 +3490,28 @@
       <c r="D13" s="27">
         <v>1</v>
       </c>
-      <c r="E13" s="63">
+      <c r="E13" s="44">
         <v>1</v>
       </c>
       <c r="F13" s="32"/>
       <c r="G13" s="27">
         <v>0.33329999999999999</v>
       </c>
-      <c r="H13" s="63">
+      <c r="H13" s="44">
         <v>1</v>
       </c>
       <c r="I13" s="32"/>
-      <c r="K13" s="78">
-        <v>1</v>
-      </c>
-      <c r="L13" s="79">
-        <v>1</v>
-      </c>
-      <c r="M13" s="78">
-        <v>1</v>
-      </c>
-      <c r="N13" s="79">
-        <v>1</v>
+      <c r="K13" s="53">
+        <v>1</v>
+      </c>
+      <c r="L13" s="54">
+        <v>1</v>
+      </c>
+      <c r="M13" s="53">
+        <v>1</v>
+      </c>
+      <c r="N13" s="54">
+        <v>0.13639999999999999</v>
       </c>
     </row>
     <row r="14" spans="2:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -3497,58 +3519,56 @@
         <f>AVERAGE(D5:D13)</f>
         <v>0.77777777777777779</v>
       </c>
-      <c r="E14" s="64">
+      <c r="E14" s="45">
         <f t="shared" ref="E14:F14" si="0">AVERAGE(E5:E13)</f>
         <v>0.22222222222222221</v>
       </c>
-      <c r="F14" s="38" t="e">
+      <c r="F14" s="38">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="G14" s="34">
         <f>AVERAGE(G5:G13)</f>
         <v>0.13703333333333334</v>
       </c>
-      <c r="H14" s="64">
+      <c r="H14" s="45">
         <f t="shared" ref="H14:I14" si="1">AVERAGE(H5:H13)</f>
         <v>0.22222222222222221</v>
       </c>
-      <c r="I14" s="38" t="e">
+      <c r="I14" s="38">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K14" s="80">
+        <v>0.16350000000000001</v>
+      </c>
+      <c r="K14" s="55">
         <f t="shared" ref="K14:L14" si="2">AVERAGE(K5:K13)</f>
         <v>0.8666666666666667</v>
       </c>
-      <c r="L14" s="81">
+      <c r="L14" s="56">
         <f t="shared" si="2"/>
         <v>0.65370000000000006</v>
       </c>
-      <c r="M14" s="80">
-        <f t="shared" ref="M14:N14" si="3">AVERAGE(M5:M13)</f>
-        <v>0.8666666666666667</v>
-      </c>
-      <c r="N14" s="81">
-        <f t="shared" si="3"/>
-        <v>0.65370000000000006</v>
+      <c r="M14" s="55">
+        <v>1</v>
+      </c>
+      <c r="N14" s="56">
+        <v>0.63263333333333327</v>
       </c>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="C17" s="55" t="s">
+      <c r="C17" s="73" t="s">
         <v>59</v>
       </c>
-      <c r="D17" s="55"/>
-      <c r="E17" s="55" t="s">
+      <c r="D17" s="73"/>
+      <c r="E17" s="73" t="s">
         <v>66</v>
       </c>
-      <c r="F17" s="55"/>
-      <c r="G17" s="55"/>
-      <c r="H17" s="55"/>
-      <c r="I17" s="55"/>
-      <c r="J17" s="55"/>
-      <c r="K17" s="55"/>
-      <c r="L17" s="55"/>
+      <c r="F17" s="73"/>
+      <c r="G17" s="73"/>
+      <c r="H17" s="73"/>
+      <c r="I17" s="73"/>
+      <c r="J17" s="73"/>
+      <c r="K17" s="73"/>
+      <c r="L17" s="73"/>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B18" s="14" t="s">
@@ -3825,14 +3845,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="K1:N1"/>
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="E17:L17"/>
     <mergeCell ref="D3:F3"/>
     <mergeCell ref="G3:I3"/>
     <mergeCell ref="D2:I2"/>
     <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="K1:N1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
create base line solr
</commit_message>
<xml_diff>
--- a/hammer-colombo/fuzzy-examples-set/test.xlsx
+++ b/hammer-colombo/fuzzy-examples-set/test.xlsx
@@ -3058,7 +3058,7 @@
   <dimension ref="B1:T29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3323,14 +3323,18 @@
       <c r="E8" s="43">
         <v>0</v>
       </c>
-      <c r="F8" s="10"/>
+      <c r="F8" s="10">
+        <v>1</v>
+      </c>
       <c r="G8" s="7">
         <v>0</v>
       </c>
       <c r="H8" s="43">
         <v>0</v>
       </c>
-      <c r="I8" s="10"/>
+      <c r="I8" s="10">
+        <v>0.33329999999999999</v>
+      </c>
       <c r="K8" s="51">
         <v>0.66669999999999996</v>
       </c>
@@ -3537,7 +3541,7 @@
       </c>
       <c r="I14" s="38">
         <f t="shared" si="1"/>
-        <v>0.16350000000000001</v>
+        <v>0.20595000000000002</v>
       </c>
       <c r="K14" s="55">
         <f t="shared" ref="K14:L14" si="2">AVERAGE(K5:K13)</f>

</xml_diff>

<commit_message>
create baseline with apache solr
</commit_message>
<xml_diff>
--- a/hammer-colombo/fuzzy-examples-set/test.xlsx
+++ b/hammer-colombo/fuzzy-examples-set/test.xlsx
@@ -3058,7 +3058,7 @@
   <dimension ref="B1:T29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3437,14 +3437,18 @@
       <c r="E11" s="43">
         <v>0</v>
       </c>
-      <c r="F11" s="10"/>
+      <c r="F11" s="10">
+        <v>1</v>
+      </c>
       <c r="G11" s="7">
         <v>0.2</v>
       </c>
       <c r="H11" s="43">
         <v>0</v>
       </c>
-      <c r="I11" s="10"/>
+      <c r="I11" s="10">
+        <v>0.16669999999999999</v>
+      </c>
       <c r="K11" s="51">
         <v>1</v>
       </c>
@@ -3549,7 +3553,7 @@
       </c>
       <c r="I14" s="38">
         <f t="shared" si="1"/>
-        <v>0.32063333333333338</v>
+        <v>0.29864285714285715</v>
       </c>
       <c r="K14" s="55">
         <f t="shared" ref="K14:L14" si="2">AVERAGE(K5:K13)</f>

</xml_diff>